<commit_message>
project with specflow feature file
</commit_message>
<xml_diff>
--- a/Keys_Onboarding/ExcelData/TestData.xlsx
+++ b/Keys_Onboarding/ExcelData/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B62415-561F-49A7-AABE-C9C0C3AA9CD8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971F518E-0AB7-4E22-B0F9-9C69D65DB981}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14505" windowHeight="6315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Url</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>abc1abc1</t>
+  </si>
+  <si>
+    <t>baha.godbole@gmail.com</t>
+  </si>
+  <si>
+    <t>description added</t>
   </si>
 </sst>
 </file>
@@ -375,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,13 +423,29 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{8D12DA7E-150E-435F-A6DB-84D6E3A372F2}"/>
+    <hyperlink ref="A3" r:id="rId4" xr:uid="{A7DD2173-0644-4CD0-8727-F8F9A4999EA8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>